<commit_message>
Tesztelés folyamat dokumentáció módosítás
</commit_message>
<xml_diff>
--- a/Tesztdokumentáció/Elvégzett tesztek/Komponensek-Unit tesztek/4.xlsx
+++ b/Tesztdokumentáció/Elvégzett tesztek/Komponensek-Unit tesztek/4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\március\Projketlab2019-03-22\Projlab2019lev\Tesztdokumentáció\Elvégzett tesztek\Komponensek-Unit tesztek\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Tesztadat:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Kilépési feltétel:</t>
   </si>
@@ -35,9 +32,6 @@
     <t>Teszt tárgya:</t>
   </si>
   <si>
-    <t>Tesztbázis:</t>
-  </si>
-  <si>
     <t>Teszt időpontja:</t>
   </si>
   <si>
@@ -57,6 +51,12 @@
   </si>
   <si>
     <t>http://www.mintantermunk.nhely.hu/web/index.htm</t>
+  </si>
+  <si>
+    <t>2019.05.14-16</t>
+  </si>
+  <si>
+    <t>Tesztlépés:</t>
   </si>
 </sst>
 </file>
@@ -81,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -90,9 +90,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -105,12 +135,81 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -120,10 +219,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -135,82 +258,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -228,24 +291,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -526,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,78 +612,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="8">
-        <v>43599</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="11"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="11"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="12"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="D2:D7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>